<commit_message>
Weight results from corrosion process
</commit_message>
<xml_diff>
--- a/RebarDataBase.xlsx
+++ b/RebarDataBase.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Label</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t>Measured Corrosion Level</t>
+  </si>
+  <si>
+    <t>CL20-T-G80</t>
+  </si>
+  <si>
+    <t>CL20-BBT-1-3-G80</t>
+  </si>
+  <si>
+    <t>CL20-BBT-4-6-G80</t>
+  </si>
+  <si>
+    <t>CL25-T-G80</t>
+  </si>
+  <si>
+    <t>CL25-BBT-1-3-G80</t>
+  </si>
+  <si>
+    <t>CL25-BBT-4-6-G80</t>
   </si>
 </sst>
 </file>
@@ -205,7 +223,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,8 +236,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -245,12 +287,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -270,41 +352,125 @@
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="O35" sqref="O35:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,908 +831,1482 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="20">
         <f>8/10+19*0.001</f>
         <v>0.81900000000000006</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="21">
         <f>+AVERAGE(B2:B4)</f>
         <v>0.81500000000000006</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="21">
         <f>50+7/8</f>
         <v>50.875</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="21">
         <v>6.1524999999999999</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="22">
         <f>+G2*12</f>
         <v>1.4512039312039311</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="22">
         <f>+E2/D2</f>
         <v>0.12093366093366092</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="22">
         <f>0.25*PI()*C2^2*D2</f>
         <v>26.540525712330844</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="22">
         <f>+E2/H2</f>
         <v>0.23181530263138389</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="23">
         <f>+I2*12^3</f>
         <v>400.57684294703137</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="21">
         <v>6.4095000000000004</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="24">
         <f>ROUND(G2*21*0.05,4)</f>
         <v>0.127</v>
       </c>
-      <c r="M2" s="20">
+      <c r="M2" s="25">
         <v>6.27</v>
       </c>
-      <c r="N2" s="20">
+      <c r="N2" s="25">
         <f>+K2-M2</f>
         <v>0.13950000000000085</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="1">
-        <v>0.81399999999999995</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="14">
-        <v>6.4095000000000004</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="23">
+      <c r="O2" s="48">
         <f>+N2/(G2*21)</f>
         <v>5.4929761421025472E-2</v>
       </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="28">
+        <v>6.4095000000000004</v>
+      </c>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="49"/>
       <c r="P3" s="1"/>
-      <c r="U3" s="22"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="1">
+      <c r="U3" s="15"/>
+    </row>
+    <row r="4" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27">
         <v>0.81200000000000006</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="14">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="28">
         <v>6</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="12"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="49"/>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="27">
         <v>0.79400000000000004</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="29">
         <f>+AVERAGE(B5:B7)</f>
         <v>0.80833333333333324</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="28">
         <f>51+1/8</f>
         <v>51.125</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="28">
         <v>6.1509999999999998</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="29">
         <f t="shared" ref="F5" si="0">+G5*12</f>
         <v>1.4437555012224939</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="29">
         <f t="shared" ref="G5" si="1">+E5/D5</f>
         <v>0.12031295843520783</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="29">
         <f t="shared" ref="H5" si="2">0.25*PI()*C5^2*D5</f>
         <v>26.23639609060152</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="29">
         <f t="shared" ref="I5" si="3">+E5/H5</f>
         <v>0.23444530943803785</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="30">
         <f t="shared" ref="J5" si="4">+I5*12^3</f>
         <v>405.12149470892939</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="28">
         <v>6.3849999999999998</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="31">
         <f t="shared" ref="L5" si="5">ROUND(G5*21*0.05,4)</f>
         <v>0.1263</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="18">
+      <c r="M5" s="32">
+        <v>6.2750000000000004</v>
+      </c>
+      <c r="N5" s="25">
         <f t="shared" ref="N5" si="6">+K5-M5</f>
-        <v>6.3849999999999998</v>
-      </c>
-      <c r="O5" s="11"/>
+        <v>0.10999999999999943</v>
+      </c>
+      <c r="O5" s="48">
+        <f t="shared" ref="O5" si="7">+N5/(G5*21)</f>
+        <v>4.3537249072934103E-2</v>
+      </c>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="1">
+      <c r="A6" s="26"/>
+      <c r="B6" s="27">
         <v>0.81599999999999995</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="11"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="49"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="1">
+    <row r="7" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27">
         <v>0.81499999999999995</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="11"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="49"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="27">
         <v>0.84799999999999998</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="29">
         <f>+AVERAGE(B8:B10)</f>
         <v>0.80133333333333334</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="28">
         <f>51+1/16</f>
         <v>51.0625</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="28">
         <v>6.16</v>
       </c>
-      <c r="F8" s="16">
-        <f t="shared" ref="F8" si="7">+G8*12</f>
+      <c r="F8" s="29">
+        <f t="shared" ref="F8" si="8">+G8*12</f>
         <v>1.4476376988984088</v>
       </c>
-      <c r="G8" s="16">
-        <f t="shared" ref="G8" si="8">+E8/D8</f>
+      <c r="G8" s="29">
+        <f t="shared" ref="G8" si="9">+E8/D8</f>
         <v>0.12063647490820073</v>
       </c>
-      <c r="H8" s="16">
-        <f t="shared" ref="H8" si="9">0.25*PI()*C8^2*D8</f>
+      <c r="H8" s="29">
+        <f t="shared" ref="H8" si="10">0.25*PI()*C8^2*D8</f>
         <v>25.752439316461313</v>
       </c>
-      <c r="I8" s="16">
-        <f t="shared" ref="I8" si="10">+E8/H8</f>
+      <c r="I8" s="29">
+        <f t="shared" ref="I8" si="11">+E8/H8</f>
         <v>0.23920064131798355</v>
       </c>
-      <c r="J8" s="15">
-        <f t="shared" ref="J8" si="11">+I8*12^3</f>
+      <c r="J8" s="30">
+        <f t="shared" ref="J8" si="12">+I8*12^3</f>
         <v>413.33870819747557</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="28">
         <v>6.3975</v>
       </c>
-      <c r="L8" s="13">
-        <f t="shared" ref="L8" si="12">ROUND(G8*21*0.05,4)</f>
+      <c r="L8" s="31">
+        <f t="shared" ref="L8" si="13">ROUND(G8*21*0.05,4)</f>
         <v>0.12670000000000001</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="18">
-        <f t="shared" ref="N8" si="13">+K8-M8</f>
-        <v>6.3975</v>
-      </c>
-      <c r="O8" s="11"/>
+      <c r="M8" s="32">
+        <v>6.2450000000000001</v>
+      </c>
+      <c r="N8" s="25">
+        <f t="shared" ref="N8" si="14">+K8-M8</f>
+        <v>0.15249999999999986</v>
+      </c>
+      <c r="O8" s="48">
+        <f t="shared" ref="O8" si="15">+N8/(G8*21)</f>
+        <v>6.0196592841682071E-2</v>
+      </c>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="1">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27">
         <v>0.73599999999999999</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="11"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="49"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="1">
+    <row r="10" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27">
         <v>0.82</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="11"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="49"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="27">
         <v>0.79400000000000004</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="28">
         <f>+AVERAGE(B11:B13)</f>
         <v>0.79900000000000004</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="28">
         <f>51+1/8</f>
         <v>51.125</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="28">
         <v>6.1740000000000004</v>
       </c>
-      <c r="F11" s="16">
-        <f t="shared" ref="F11" si="14">+G11*12</f>
+      <c r="F11" s="29">
+        <f t="shared" ref="F11" si="16">+G11*12</f>
         <v>1.449154034229829</v>
       </c>
-      <c r="G11" s="16">
-        <f t="shared" ref="G11" si="15">+E11/D11</f>
+      <c r="G11" s="29">
+        <f t="shared" ref="G11" si="17">+E11/D11</f>
         <v>0.12076283618581908</v>
       </c>
-      <c r="H11" s="16">
-        <f t="shared" ref="H11" si="16">0.25*PI()*C11^2*D11</f>
+      <c r="H11" s="29">
+        <f t="shared" ref="H11" si="18">0.25*PI()*C11^2*D11</f>
         <v>25.634022490079705</v>
       </c>
-      <c r="I11" s="16">
-        <f t="shared" ref="I11" si="17">+E11/H11</f>
+      <c r="I11" s="29">
+        <f t="shared" ref="I11" si="19">+E11/H11</f>
         <v>0.24085178213404942</v>
       </c>
-      <c r="J11" s="15">
-        <f t="shared" ref="J11" si="18">+I11*12^3</f>
+      <c r="J11" s="30">
+        <f t="shared" ref="J11" si="20">+I11*12^3</f>
         <v>416.19187952763741</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="28">
         <v>6.3724999999999996</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="31">
         <f>ROUND(G11*21*0.1,4)</f>
         <v>0.25359999999999999</v>
       </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="18">
-        <f t="shared" ref="N11" si="19">+K11-M11</f>
-        <v>6.3724999999999996</v>
-      </c>
-      <c r="O11" s="11"/>
+      <c r="M11" s="32">
+        <v>6.1050000000000004</v>
+      </c>
+      <c r="N11" s="25">
+        <f t="shared" ref="N11" si="21">+K11-M11</f>
+        <v>0.26749999999999918</v>
+      </c>
+      <c r="O11" s="50">
+        <f t="shared" ref="O11" si="22">+N11/(G11*21)</f>
+        <v>0.10548025899702251</v>
+      </c>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27">
         <v>0.80500000000000005</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="11"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="1">
+    <row r="13" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27">
         <v>0.79800000000000004</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="11"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="51"/>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="27">
         <v>0.81399999999999995</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="28">
         <f>+AVERAGE(B14:B16)</f>
         <v>0.80100000000000005</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="28">
         <v>51</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="28">
         <v>6.4390000000000001</v>
       </c>
-      <c r="F14" s="16">
-        <f t="shared" ref="F14" si="20">+G14*12</f>
+      <c r="F14" s="29">
+        <f t="shared" ref="F14" si="23">+G14*12</f>
         <v>1.5150588235294118</v>
       </c>
-      <c r="G14" s="16">
-        <f t="shared" ref="G14" si="21">+E14/D14</f>
+      <c r="G14" s="29">
+        <f t="shared" ref="G14" si="24">+E14/D14</f>
         <v>0.12625490196078432</v>
       </c>
-      <c r="H14" s="16">
-        <f t="shared" ref="H14" si="22">0.25*PI()*C14^2*D14</f>
+      <c r="H14" s="29">
+        <f t="shared" ref="H14" si="25">0.25*PI()*C14^2*D14</f>
         <v>25.699524598732282</v>
       </c>
-      <c r="I14" s="16">
-        <f t="shared" ref="I14" si="23">+E14/H14</f>
+      <c r="I14" s="29">
+        <f t="shared" ref="I14" si="26">+E14/H14</f>
         <v>0.25054938177018365</v>
       </c>
-      <c r="J14" s="15">
-        <f t="shared" ref="J14" si="24">+I14*12^3</f>
+      <c r="J14" s="30">
+        <f t="shared" ref="J14" si="27">+I14*12^3</f>
         <v>432.94933169887736</v>
       </c>
-      <c r="K14" s="14">
-        <v>3.3919999999999999</v>
-      </c>
-      <c r="L14" s="13">
-        <f t="shared" ref="L14" si="25">ROUND(G14*21*0.1,4)</f>
+      <c r="K14" s="28">
+        <v>6.3920000000000003</v>
+      </c>
+      <c r="L14" s="31">
+        <f t="shared" ref="L14" si="28">ROUND(G14*21*0.1,4)</f>
         <v>0.2651</v>
       </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="18">
-        <f t="shared" ref="N14" si="26">+K14-M14</f>
-        <v>3.3919999999999999</v>
-      </c>
-      <c r="O14" s="11"/>
+      <c r="M14" s="32">
+        <v>6.32</v>
+      </c>
+      <c r="N14" s="25">
+        <f t="shared" ref="N14" si="29">+K14-M14</f>
+        <v>7.2000000000000064E-2</v>
+      </c>
+      <c r="O14" s="48">
+        <f t="shared" ref="O14" si="30">+N14/(G14*21)</f>
+        <v>2.7155947019279859E-2</v>
+      </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="1">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27">
         <v>0.79600000000000004</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="11"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="49"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="1">
+    <row r="16" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27">
         <v>0.79300000000000004</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="11"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="49"/>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="27">
         <v>0.84899999999999998</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="28">
         <f>+AVERAGE(B17:B19)</f>
         <v>0.83</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="28">
         <v>51</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="28">
         <v>6.1260000000000003</v>
       </c>
-      <c r="F17" s="16">
-        <f t="shared" ref="F17" si="27">+G17*12</f>
+      <c r="F17" s="29">
+        <f t="shared" ref="F17" si="31">+G17*12</f>
         <v>1.4414117647058824</v>
       </c>
-      <c r="G17" s="16">
-        <f t="shared" ref="G17" si="28">+E17/D17</f>
+      <c r="G17" s="29">
+        <f t="shared" ref="G17" si="32">+E17/D17</f>
         <v>0.12011764705882354</v>
       </c>
-      <c r="H17" s="16">
-        <f t="shared" ref="H17" si="29">0.25*PI()*C17^2*D17</f>
+      <c r="H17" s="29">
+        <f t="shared" ref="H17" si="33">0.25*PI()*C17^2*D17</f>
         <v>27.594100532989607</v>
       </c>
-      <c r="I17" s="16">
-        <f t="shared" ref="I17" si="30">+E17/H17</f>
+      <c r="I17" s="29">
+        <f t="shared" ref="I17" si="34">+E17/H17</f>
         <v>0.22200397482339301</v>
       </c>
-      <c r="J17" s="15">
-        <f t="shared" ref="J17" si="31">+I17*12^3</f>
+      <c r="J17" s="30">
+        <f t="shared" ref="J17" si="35">+I17*12^3</f>
         <v>383.62286849482314</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="28">
         <v>6.383</v>
       </c>
-      <c r="L17" s="13">
-        <f t="shared" ref="L17" si="32">ROUND(G17*21*0.1,4)</f>
+      <c r="L17" s="31">
+        <f t="shared" ref="L17" si="36">ROUND(G17*21*0.1,4)</f>
         <v>0.25219999999999998</v>
       </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="18">
-        <f t="shared" ref="N17" si="33">+K17-M17</f>
-        <v>6.383</v>
-      </c>
-      <c r="O17" s="11"/>
+      <c r="M17" s="32">
+        <v>6.07</v>
+      </c>
+      <c r="N17" s="25">
+        <f t="shared" ref="N17" si="37">+K17-M17</f>
+        <v>0.31299999999999972</v>
+      </c>
+      <c r="O17" s="50">
+        <f t="shared" ref="O17" si="38">+N17/(G17*21)</f>
+        <v>0.12408469754209213</v>
+      </c>
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27">
         <v>0.82099999999999995</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="11"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="51"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="1">
+    <row r="19" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27">
         <v>0.82</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="11"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="51"/>
       <c r="P19" s="1"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="27">
         <v>0.8</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="28">
         <f>+AVERAGE(B20:B22)</f>
         <v>0.79500000000000004</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="28">
         <f>51+1/16</f>
         <v>51.0625</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="28">
         <v>6.1505000000000001</v>
       </c>
-      <c r="F20" s="16">
-        <f t="shared" ref="F20" si="34">+G20*12</f>
+      <c r="F20" s="29">
+        <f t="shared" ref="F20" si="39">+G20*12</f>
         <v>1.4454051407588739</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" ref="G20" si="35">+E20/D20</f>
+      <c r="G20" s="29">
+        <f t="shared" ref="G20" si="40">+E20/D20</f>
         <v>0.12045042839657283</v>
       </c>
-      <c r="H20" s="16">
-        <f t="shared" ref="H20" si="36">0.25*PI()*C20^2*D20</f>
+      <c r="H20" s="29">
+        <f t="shared" ref="H20" si="41">0.25*PI()*C20^2*D20</f>
         <v>25.346979439923714</v>
       </c>
-      <c r="I20" s="16">
-        <f t="shared" ref="I20" si="37">+E20/H20</f>
+      <c r="I20" s="29">
+        <f t="shared" ref="I20" si="42">+E20/H20</f>
         <v>0.24265218719956916</v>
       </c>
-      <c r="J20" s="15">
-        <f t="shared" ref="J20" si="38">+I20*12^3</f>
+      <c r="J20" s="30">
+        <f t="shared" ref="J20" si="43">+I20*12^3</f>
         <v>419.30297948085553</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="28">
         <v>6.3884999999999996</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="31">
         <f>ROUND(G20*21*0.15,4)</f>
         <v>0.37940000000000002</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="18">
-        <f t="shared" ref="N20" si="39">+K20-M20</f>
-        <v>6.3884999999999996</v>
-      </c>
-      <c r="O20" s="11"/>
+      <c r="M20" s="32">
+        <v>5.8849999999999998</v>
+      </c>
+      <c r="N20" s="25">
+        <f t="shared" ref="N20" si="44">+K20-M20</f>
+        <v>0.50349999999999984</v>
+      </c>
+      <c r="O20" s="52">
+        <f t="shared" ref="O20" si="45">+N20/(G20*21)</f>
+        <v>0.1990544225982401</v>
+      </c>
       <c r="P20" s="1"/>
     </row>
     <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="27">
         <v>0.79</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="11"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="53"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="1">
+    <row r="22" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27">
         <v>0.79500000000000004</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="11"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="53"/>
       <c r="P22" s="1"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="27">
         <v>0.79600000000000004</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="28">
         <f>+AVERAGE(B23:B25)</f>
         <v>0.79900000000000004</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="28">
         <f>51+1/16</f>
         <v>51.0625</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="28">
         <v>6.1539999999999999</v>
       </c>
-      <c r="F23" s="16">
-        <f t="shared" ref="F23" si="40">+G23*12</f>
+      <c r="F23" s="29">
+        <f t="shared" ref="F23" si="46">+G23*12</f>
         <v>1.4462276621787025</v>
       </c>
-      <c r="G23" s="16">
-        <f t="shared" ref="G23" si="41">+E23/D23</f>
+      <c r="G23" s="29">
+        <f t="shared" ref="G23" si="47">+E23/D23</f>
         <v>0.12051897184822521</v>
       </c>
-      <c r="H23" s="16">
-        <f t="shared" ref="H23" si="42">0.25*PI()*C23^2*D23</f>
+      <c r="H23" s="29">
+        <f t="shared" ref="H23" si="48">0.25*PI()*C23^2*D23</f>
         <v>25.602685054272762</v>
       </c>
-      <c r="I23" s="16">
-        <f t="shared" ref="I23" si="43">+E23/H23</f>
+      <c r="I23" s="29">
+        <f t="shared" ref="I23" si="49">+E23/H23</f>
         <v>0.24036541428973973</v>
       </c>
-      <c r="J23" s="15">
-        <f t="shared" ref="J23" si="44">+I23*12^3</f>
+      <c r="J23" s="30">
+        <f t="shared" ref="J23" si="50">+I23*12^3</f>
         <v>415.35143589267028</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="28">
         <v>6.4050000000000002</v>
       </c>
-      <c r="L23" s="13">
-        <f t="shared" ref="L23" si="45">ROUND(G23*21*0.15,4)</f>
+      <c r="L23" s="31">
+        <f t="shared" ref="L23" si="51">ROUND(G23*21*0.15,4)</f>
         <v>0.37959999999999999</v>
       </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="18">
-        <f t="shared" ref="N23" si="46">+K23-M23</f>
-        <v>6.4050000000000002</v>
-      </c>
-      <c r="O23" s="11"/>
+      <c r="M23" s="32">
+        <v>6.125</v>
+      </c>
+      <c r="N23" s="25">
+        <f t="shared" ref="N23" si="52">+K23-M23</f>
+        <v>0.28000000000000025</v>
+      </c>
+      <c r="O23" s="50">
+        <f t="shared" ref="O23" si="53">+N23/(G23*21)</f>
+        <v>0.1106326508503955</v>
+      </c>
       <c r="P23" s="1"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="1">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27">
         <v>0.78700000000000003</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="11"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="51"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="1">
+    <row r="25" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="27">
         <v>0.81399999999999995</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="11"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="51"/>
       <c r="P25" s="1"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="27">
         <v>0.81899999999999995</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="28">
         <f>+AVERAGE(B26:B28)</f>
         <v>0.80799999999999994</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="28">
         <v>51</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="28">
         <v>6.1459999999999999</v>
       </c>
-      <c r="F26" s="16">
-        <f t="shared" ref="F26" si="47">+G26*12</f>
+      <c r="F26" s="29">
+        <f t="shared" ref="F26" si="54">+G26*12</f>
         <v>1.4461176470588235</v>
       </c>
-      <c r="G26" s="16">
-        <f t="shared" ref="G26" si="48">+E26/D26</f>
+      <c r="G26" s="29">
+        <f>+E26/D26</f>
         <v>0.12050980392156863</v>
       </c>
-      <c r="H26" s="16">
-        <f t="shared" ref="H26" si="49">0.25*PI()*C26^2*D26</f>
+      <c r="H26" s="29">
+        <f t="shared" ref="H26" si="55">0.25*PI()*C26^2*D26</f>
         <v>26.150667513963892</v>
       </c>
-      <c r="I26" s="16">
-        <f t="shared" ref="I26" si="50">+E26/H26</f>
+      <c r="I26" s="29">
+        <f t="shared" ref="I26" si="56">+E26/H26</f>
         <v>0.23502268141790905</v>
       </c>
-      <c r="J26" s="15">
-        <f t="shared" ref="J26" si="51">+I26*12^3</f>
+      <c r="J26" s="30">
+        <f t="shared" ref="J26" si="57">+I26*12^3</f>
         <v>406.11919349014681</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="28">
         <v>6.4015000000000004</v>
       </c>
-      <c r="L26" s="13">
-        <f t="shared" ref="L26" si="52">ROUND(G26*21*0.15,4)</f>
+      <c r="L26" s="31">
+        <f t="shared" ref="L26" si="58">ROUND(G26*21*0.15,4)</f>
         <v>0.37959999999999999</v>
       </c>
-      <c r="M26" s="19"/>
-      <c r="N26" s="18">
-        <f t="shared" ref="N26" si="53">+K26-M26</f>
-        <v>6.4015000000000004</v>
-      </c>
-      <c r="O26" s="11"/>
+      <c r="M26" s="32">
+        <v>6.16</v>
+      </c>
+      <c r="N26" s="25">
+        <f t="shared" ref="N26" si="59">+K26-M26</f>
+        <v>0.24150000000000027</v>
+      </c>
+      <c r="O26" s="50">
+        <f>+N26/(G26*21)</f>
+        <v>9.5427920598763538E-2</v>
+      </c>
       <c r="P26" s="1"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="1">
+      <c r="A27" s="26"/>
+      <c r="B27" s="27">
         <v>0.79100000000000004</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="12"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="51"/>
       <c r="P27" s="1"/>
     </row>
     <row r="28" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="17"/>
-      <c r="B28" s="1">
+      <c r="A28" s="26"/>
+      <c r="B28" s="27">
         <v>0.81399999999999995</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="12"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="51"/>
       <c r="P28" s="1"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="28">
+        <v>6.375</v>
+      </c>
+      <c r="L29" s="31">
+        <f>ROUND(G29*21*0.2,4)</f>
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="M29" s="32">
+        <v>5.875</v>
+      </c>
+      <c r="N29" s="25">
+        <f t="shared" ref="N29:N44" si="60">+K29-M29</f>
+        <v>0.5</v>
+      </c>
+      <c r="O29" s="52">
+        <f>+N29/(G29*21)</f>
+        <v>0.19677292404565133</v>
+      </c>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="53"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="28">
+        <v>6.4349999999999996</v>
+      </c>
+      <c r="L32" s="31">
+        <f t="shared" ref="L32:L40" si="61">ROUND(G32*21*0.2,4)</f>
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="M32" s="32">
+        <v>5.8650000000000002</v>
+      </c>
+      <c r="N32" s="25">
+        <f t="shared" si="60"/>
+        <v>0.5699999999999994</v>
+      </c>
+      <c r="O32" s="52">
+        <f t="shared" ref="O32" si="62">+N32/(G32*21)</f>
+        <v>0.22432113341204227</v>
+      </c>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="53"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="53"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="28">
+        <v>6.375</v>
+      </c>
+      <c r="L35" s="31">
+        <f t="shared" ref="L35:L40" si="63">ROUND(G35*21*0.2,4)</f>
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="M35" s="32">
+        <v>6.1550000000000002</v>
+      </c>
+      <c r="N35" s="25">
+        <f t="shared" si="60"/>
+        <v>0.21999999999999975</v>
+      </c>
+      <c r="O35" s="50">
+        <f t="shared" ref="O35" si="64">+N35/(G35*21)</f>
+        <v>8.6580086580086479E-2</v>
+      </c>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="28">
+        <v>6.4649999999999999</v>
+      </c>
+      <c r="L38" s="31">
+        <f>ROUND(G38*21*0.25,4)</f>
+        <v>0.63529999999999998</v>
+      </c>
+      <c r="M38" s="32">
+        <v>5.93</v>
+      </c>
+      <c r="N38" s="25">
+        <f t="shared" si="60"/>
+        <v>0.53500000000000014</v>
+      </c>
+      <c r="O38" s="52">
+        <f t="shared" ref="O38" si="65">+N38/(G38*21)</f>
+        <v>0.21054702872884698</v>
+      </c>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="53"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="28">
+        <v>6.3150000000000004</v>
+      </c>
+      <c r="L41" s="31">
+        <f t="shared" ref="L41:L46" si="66">ROUND(G41*21*0.25,4)</f>
+        <v>0.63529999999999998</v>
+      </c>
+      <c r="M41" s="32">
+        <v>5.95</v>
+      </c>
+      <c r="N41" s="25">
+        <f t="shared" si="60"/>
+        <v>0.36500000000000021</v>
+      </c>
+      <c r="O41" s="46">
+        <f t="shared" ref="O41" si="67">+N41/(G41*21)</f>
+        <v>0.14364423455332556</v>
+      </c>
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="43">
+        <v>0.121</v>
+      </c>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="18">
+        <v>6.42</v>
+      </c>
+      <c r="L44" s="31">
+        <f t="shared" ref="L44:L46" si="68">ROUND(G44*21*0.25,4)</f>
+        <v>0.63529999999999998</v>
+      </c>
+      <c r="M44" s="16">
+        <v>5.9850000000000003</v>
+      </c>
+      <c r="N44" s="25">
+        <f t="shared" si="60"/>
+        <v>0.43499999999999961</v>
+      </c>
+      <c r="O44" s="46">
+        <f t="shared" ref="O44" si="69">+N44/(G44*21)</f>
+        <v>0.1711924439197165</v>
+      </c>
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="17"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="47"/>
+      <c r="P46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3">
+      <c r="B47" s="2"/>
+      <c r="C47" s="3">
         <f>AVERAGE(C2:C28)</f>
         <v>0.80629629629629629</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D47" s="3">
         <f>AVERAGE(D2:D28)</f>
         <v>51.034722222222221</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E47" s="3">
         <f>AVERAGE(E2:E28)</f>
         <v>6.1836666666666673</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F47" s="3">
         <f>AVERAGE(F2:F28)</f>
         <v>1.4539969115318172</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="4">
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="4">
         <f>AVERAGE(J2:J28)</f>
         <v>410.28608160427189</v>
       </c>
-      <c r="K29" s="3">
-        <f>AVERAGE(K2:K28)</f>
-        <v>6.0858181818181833</v>
-      </c>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
+      <c r="K47" s="3">
+        <f>AVERAGE(K2:K46)</f>
+        <v>6.3722941176470602</v>
+      </c>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="117">
-    <mergeCell ref="N17:N19"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="M11:M13"/>
-    <mergeCell ref="M14:M16"/>
-    <mergeCell ref="M17:M19"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="N11:N13"/>
-    <mergeCell ref="N14:N16"/>
+  <mergeCells count="168">
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="L38:L40"/>
+    <mergeCell ref="L41:L43"/>
+    <mergeCell ref="L44:L46"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="O8:O10"/>
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="O14:O16"/>
+    <mergeCell ref="O17:O19"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="O29:O31"/>
+    <mergeCell ref="O32:O34"/>
+    <mergeCell ref="O35:O37"/>
+    <mergeCell ref="O38:O40"/>
+    <mergeCell ref="O41:O43"/>
+    <mergeCell ref="O44:O46"/>
+    <mergeCell ref="N29:N31"/>
+    <mergeCell ref="N32:N34"/>
+    <mergeCell ref="N35:N37"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="N41:N43"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="M29:M31"/>
+    <mergeCell ref="M32:M34"/>
+    <mergeCell ref="M35:M37"/>
+    <mergeCell ref="M38:M40"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="M44:M45"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K32:K34"/>
+    <mergeCell ref="K35:K37"/>
+    <mergeCell ref="K38:K40"/>
+    <mergeCell ref="K41:K43"/>
+    <mergeCell ref="K44:K46"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="L26:L28"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="K20:K22"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="K8:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A28"/>
@@ -1589,83 +2329,26 @@
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="L26:L28"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="K20:K22"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="K26:K28"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="N17:N19"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="M11:M13"/>
+    <mergeCell ref="M14:M16"/>
+    <mergeCell ref="M17:M19"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="N11:N13"/>
+    <mergeCell ref="N14:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1713,7 +2396,7 @@
         <v>0.75</v>
       </c>
       <c r="C2" s="9">
-        <f>+Sheet1!C29</f>
+        <f>+Sheet1!C47</f>
         <v>0.80629629629629629</v>
       </c>
       <c r="D2" s="10">
@@ -1732,7 +2415,7 @@
         <v>1.502</v>
       </c>
       <c r="C3" s="9">
-        <f>+Sheet1!F29</f>
+        <f>+Sheet1!F47</f>
         <v>1.4539969115318172</v>
       </c>
       <c r="D3" s="10">

</xml_diff>